<commit_message>
Update template files for req, design, test case
-Update templates for req, design, test
</commit_message>
<xml_diff>
--- a/Requirement/AUTOSAR_SWS_ADCDriver.xlsx
+++ b/Requirement/AUTOSAR_SWS_ADCDriver.xlsx
@@ -1,23 +1,204 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Requirement Identifier unique for each new line</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Type of requirement functional or non functional</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Status of implementation
+OPEN, NA, CLOSED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mention the linked Test Case ID and document name with version number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mention the linked Design ID and document name with version number</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Review status , INREVIEW, COMPLETED, FORREVIEW, OPEN</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>ReqID</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>TestCase ID</t>
+  </si>
+  <si>
+    <t>Design ID</t>
+  </si>
+  <si>
+    <t>Review Status</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,13 +206,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +254,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,13 +551,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="69" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -358,7 +603,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -370,7 +615,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>